<commit_message>
Add descriptive text for qualitative labels.
</commit_message>
<xml_diff>
--- a/survey/HITRUST Survey Document.xlsx
+++ b/survey/HITRUST Survey Document.xlsx
@@ -5,42 +5,43 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\strat-risk\survey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\evaluator\survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="9435" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="18" r:id="rId1"/>
-    <sheet name="ISMP" sheetId="1" r:id="rId2"/>
+    <sheet name="Definitions" sheetId="21" r:id="rId2"/>
     <sheet name="Reference" sheetId="14" state="hidden" r:id="rId3"/>
-    <sheet name="AC" sheetId="13" r:id="rId4"/>
-    <sheet name="HR" sheetId="7" r:id="rId5"/>
-    <sheet name="RISK" sheetId="4" r:id="rId6"/>
-    <sheet name="POL" sheetId="2" r:id="rId7"/>
-    <sheet name="ORG" sheetId="15" r:id="rId8"/>
-    <sheet name="COMP" sheetId="3" r:id="rId9"/>
-    <sheet name="ASSET" sheetId="12" r:id="rId10"/>
-    <sheet name="PHY" sheetId="11" r:id="rId11"/>
-    <sheet name="OPS" sheetId="19" r:id="rId12"/>
-    <sheet name="ADM" sheetId="16" r:id="rId13"/>
-    <sheet name="IM" sheetId="20" r:id="rId14"/>
-    <sheet name="BC" sheetId="17" r:id="rId15"/>
-    <sheet name="PRI" sheetId="5" r:id="rId16"/>
+    <sheet name="ISMP" sheetId="1" r:id="rId4"/>
+    <sheet name="AC" sheetId="13" r:id="rId5"/>
+    <sheet name="HR" sheetId="7" r:id="rId6"/>
+    <sheet name="RISK" sheetId="4" r:id="rId7"/>
+    <sheet name="POL" sheetId="2" r:id="rId8"/>
+    <sheet name="ORG" sheetId="15" r:id="rId9"/>
+    <sheet name="COMP" sheetId="3" r:id="rId10"/>
+    <sheet name="ASSET" sheetId="12" r:id="rId11"/>
+    <sheet name="PHY" sheetId="11" r:id="rId12"/>
+    <sheet name="OPS" sheetId="19" r:id="rId13"/>
+    <sheet name="ADM" sheetId="16" r:id="rId14"/>
+    <sheet name="IM" sheetId="20" r:id="rId15"/>
+    <sheet name="BC" sheetId="17" r:id="rId16"/>
+    <sheet name="PRI" sheetId="5" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
-    <definedName name="DIFF_Values" localSheetId="13">[1]Reference!$A$17:$A$21</definedName>
+    <definedName name="DIFF_Values" localSheetId="14">[1]Reference!$A$17:$A$21</definedName>
     <definedName name="DIFF_Values">Reference!$A$17:$A$21</definedName>
-    <definedName name="LM_Values" localSheetId="13">[1]Reference!$A$12:$A$14</definedName>
+    <definedName name="LM_Values" localSheetId="14">[1]Reference!$A$12:$A$14</definedName>
     <definedName name="LM_Values">Reference!$A$12:$A$14</definedName>
     <definedName name="sdfs">[1]Reference!$A$17:$A$21</definedName>
-    <definedName name="TC_Values" localSheetId="13">[1]Reference!$A$7:$A$9</definedName>
+    <definedName name="TC_Values" localSheetId="14">[1]Reference!$A$7:$A$9</definedName>
     <definedName name="TC_Values">Reference!$A$7:$A$9</definedName>
-    <definedName name="TEF_Values" localSheetId="13">[1]Reference!$A$2:$A$4</definedName>
+    <definedName name="TEF_Values" localSheetId="14">[1]Reference!$A$2:$A$4</definedName>
     <definedName name="TEF_Values">Reference!$A$2:$A$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="221">
   <si>
     <t>Threats</t>
   </si>
@@ -647,13 +648,82 @@
   </si>
   <si>
     <t>38, 44</t>
+  </si>
+  <si>
+    <t>Real and serious effect on the bottom line and/or long-term ability to generate revenue.</t>
+  </si>
+  <si>
+    <t>Significant effect on annual profit.</t>
+  </si>
+  <si>
+    <t>Opportunities for the threat to materialize many times a month.</t>
+  </si>
+  <si>
+    <t>Opportunities for the threat to materialize occur several times a year.</t>
+  </si>
+  <si>
+    <t>Opportunities for the threat to materialize occur less than once a year.</t>
+  </si>
+  <si>
+    <t>Definitions of labels</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Definitions</t>
+  </si>
+  <si>
+    <t>Lookup tables (sheet hidden by default)</t>
+  </si>
+  <si>
+    <t>Difficulty (DIFF) - Control Maturity Level (CMM)</t>
+  </si>
+  <si>
+    <t>Loss Magnitude (LM) - Size of Loss if Scenario Occurs</t>
+  </si>
+  <si>
+    <t>Threat Capability (TC) - Capability of Threat Community</t>
+  </si>
+  <si>
+    <t>Threat Expected Frequency (TEF) - Occurance of Threats Against Control</t>
+  </si>
+  <si>
+    <t>Absorbed by normal activities.</t>
+  </si>
+  <si>
+    <t>Qualitative Definitions</t>
+  </si>
+  <si>
+    <t>Actor is extremely capable. (World class)</t>
+  </si>
+  <si>
+    <t>Threat actor has typical capabilty.</t>
+  </si>
+  <si>
+    <t>Threat actor has low capability.</t>
+  </si>
+  <si>
+    <t>Optimized.</t>
+  </si>
+  <si>
+    <t>Tested and reviewed.</t>
+  </si>
+  <si>
+    <t>Considered standard practice and operational.</t>
+  </si>
+  <si>
+    <t>Repeatable and possibly consistent across the organization.</t>
+  </si>
+  <si>
+    <t>Not performed or performed inconsistently.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,13 +755,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -721,12 +811,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -748,13 +840,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title" xfId="3" builtinId="15"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="79">
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1345,11 +1470,24 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Policy_Threats" displayName="Policy_Threats" ref="A9:G12" totalsRowShown="0">
-  <autoFilter ref="A9:G12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="HR_Capabilites" displayName="HR_Capabilites" ref="A2:D6" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
+  <autoFilter ref="A2:D6"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name" dataDxfId="63"/>
+    <tableColumn id="2" name="DIFF"/>
+    <tableColumn id="5" name="Evidence"/>
+    <tableColumn id="3" name="CapabilityID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="HR_Threats" displayName="HR_Threats" ref="A9:G13" totalsRowShown="0">
+  <autoFilter ref="A9:G13"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="50"/>
-    <tableColumn id="7" name="TComm" dataDxfId="49"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="62"/>
+    <tableColumn id="7" name="TComm" dataDxfId="61"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1360,11 +1498,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Policy_Capabilities" displayName="Policy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Risk_Capabilities" displayName="Risk_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="A2:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="45"/>
+    <tableColumn id="1" name="Name" dataDxfId="57"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1373,11 +1511,56 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Risk_Threats" displayName="Risk_Threats" ref="A9:G13" totalsRowShown="0">
+  <autoFilter ref="A9:G13"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Scenario" dataDxfId="56"/>
+    <tableColumn id="7" name="TComm" dataDxfId="55"/>
+    <tableColumn id="2" name="TEF"/>
+    <tableColumn id="3" name="TC"/>
+    <tableColumn id="4" name="LM"/>
+    <tableColumn id="6" name="ScenarioID"/>
+    <tableColumn id="5" name="Capabilities"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Policy_Threats" displayName="Policy_Threats" ref="A9:G12" totalsRowShown="0">
+  <autoFilter ref="A9:G12"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Scenario" dataDxfId="54"/>
+    <tableColumn id="7" name="TComm" dataDxfId="53"/>
+    <tableColumn id="2" name="TEF"/>
+    <tableColumn id="3" name="TC"/>
+    <tableColumn id="4" name="LM"/>
+    <tableColumn id="6" name="ScenarioID"/>
+    <tableColumn id="5" name="Capabilities"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Policy_Capabilities" displayName="Policy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
+  <autoFilter ref="A2:D6"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name" dataDxfId="49"/>
+    <tableColumn id="2" name="DIFF"/>
+    <tableColumn id="5" name="Evidence"/>
+    <tableColumn id="3" name="CapabilityID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="ORG_Capabilities" displayName="ORG_Capabilities" ref="A2:D10" totalsRowShown="0">
   <autoFilter ref="A2:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="44"/>
+    <tableColumn id="1" name="Name" dataDxfId="48"/>
     <tableColumn id="4" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="2" name="CapabilityID"/>
@@ -1386,12 +1569,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="ORG_Threats" displayName="ORG_Threats" ref="A13:G18" totalsRowShown="0">
   <autoFilter ref="A13:G18"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="43"/>
-    <tableColumn id="11" name="TComm" dataDxfId="42"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="47"/>
+    <tableColumn id="11" name="TComm" dataDxfId="46"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1402,71 +1585,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="COMP_Capabilities" displayName="COMP_Capabilities" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="41"/>
+    <tableColumn id="1" name="Name" dataDxfId="45"/>
     <tableColumn id="2" name="DIFF"/>
-    <tableColumn id="5" name="Evidence" dataDxfId="40"/>
-    <tableColumn id="3" name="CapabilityID"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="COMP_Threats" displayName="COMP_Threats" ref="A7:G11" totalsRowShown="0">
-  <autoFilter ref="A7:G11"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="39"/>
-    <tableColumn id="7" name="TComm" dataDxfId="38"/>
-    <tableColumn id="2" name="TEF"/>
-    <tableColumn id="3" name="TC"/>
-    <tableColumn id="4" name="LM"/>
-    <tableColumn id="6" name="ScenarioID"/>
-    <tableColumn id="5" name="Capabilities"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Asset_Capabilities" displayName="Asset_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35">
-  <autoFilter ref="A2:D4"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="34"/>
-    <tableColumn id="2" name="DIFF"/>
-    <tableColumn id="5" name="Evidence"/>
-    <tableColumn id="3" name="CapabilityID"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Asset_Threats" displayName="Asset_Threats" ref="A8:G11" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="A8:G11"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="30"/>
-    <tableColumn id="7" name="TComm" dataDxfId="29"/>
-    <tableColumn id="2" name="TEF"/>
-    <tableColumn id="3" name="TC"/>
-    <tableColumn id="4" name="LM"/>
-    <tableColumn id="6" name="ScenarioID"/>
-    <tableColumn id="5" name="Capabilities"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Physical_Capabilities" displayName="Physical_Capabilities" ref="A2:D6" totalsRowShown="0">
-  <autoFilter ref="A2:D6"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="28"/>
-    <tableColumn id="2" name="DIFF"/>
-    <tableColumn id="5" name="Evidence"/>
+    <tableColumn id="5" name="Evidence" dataDxfId="44"/>
     <tableColumn id="3" name="CapabilityID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1474,11 +1599,11 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Physical_Threats" displayName="Physical_Threats" ref="A9:G13" totalsRowShown="0">
-  <autoFilter ref="A9:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="COMP_Threats" displayName="COMP_Threats" ref="A7:G11" totalsRowShown="0">
+  <autoFilter ref="A7:G11"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="27"/>
-    <tableColumn id="7" name="TComm" dataDxfId="26"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="43"/>
+    <tableColumn id="7" name="TComm" dataDxfId="42"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1490,23 +1615,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ISMP_Capabilities" displayName="ISMP_Capabilities" ref="A2:D5" totalsRowShown="0">
-  <autoFilter ref="A2:D5"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="74"/>
-    <tableColumn id="4" name="DIFF"/>
-    <tableColumn id="5" name="Evidence"/>
-    <tableColumn id="2" name="CapabilityID"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A4:B8" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="3">
+  <sortState ref="A4:B8">
+    <sortCondition descending="1" ref="A4:A8"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="OPS_Capabilities" displayName="OPS_Capabilities" ref="A2:D16" totalsRowShown="0">
-  <autoFilter ref="A2:D16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Asset_Capabilities" displayName="Asset_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
+  <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="25"/>
+    <tableColumn id="1" name="Name" dataDxfId="38"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1516,26 +1641,26 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="OPS_Threats" displayName="OPS_Threats" ref="A19:G27" totalsRowShown="0">
-  <autoFilter ref="A19:G27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Asset_Threats" displayName="Asset_Threats" ref="A8:G11" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35">
+  <autoFilter ref="A8:G11"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="24"/>
-    <tableColumn id="7" name="TComm" dataDxfId="23"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="34"/>
+    <tableColumn id="7" name="TComm" dataDxfId="33"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
     <tableColumn id="6" name="ScenarioID"/>
-    <tableColumn id="5" name="Capabilities" dataDxfId="22"/>
+    <tableColumn id="5" name="Capabilities"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="ADM_Capabilities" displayName="ADM_Capabilities" ref="A2:D4" totalsRowShown="0">
-  <autoFilter ref="A2:D4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Physical_Capabilities" displayName="Physical_Capabilities" ref="A2:D6" totalsRowShown="0">
+  <autoFilter ref="A2:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="21"/>
+    <tableColumn id="1" name="Name" dataDxfId="32"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1545,11 +1670,11 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="ADM_Threats" displayName="ADM_Threats" ref="A7:G8" totalsRowShown="0">
-  <autoFilter ref="A7:G8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Physical_Threats" displayName="Physical_Threats" ref="A9:G13" totalsRowShown="0">
+  <autoFilter ref="A9:G13"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="20"/>
-    <tableColumn id="7" name="TComm" dataDxfId="19"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="31"/>
+    <tableColumn id="7" name="TComm" dataDxfId="30"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1561,10 +1686,10 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="IM_Capabilities" displayName="IM_Capabilities" ref="A2:D7" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A2:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="OPS_Capabilities" displayName="OPS_Capabilities" ref="A2:D16" totalsRowShown="0">
+  <autoFilter ref="A2:D16"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="15"/>
+    <tableColumn id="1" name="Name" dataDxfId="29"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1574,26 +1699,26 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="IM_Threats" displayName="IM_Threats" ref="A10:G22" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A10:G22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="OPS_Threats" displayName="OPS_Threats" ref="A19:G27" totalsRowShown="0">
+  <autoFilter ref="A19:G27"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="11"/>
-    <tableColumn id="7" name="TComm" dataDxfId="10"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="28"/>
+    <tableColumn id="7" name="TComm" dataDxfId="27"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
     <tableColumn id="6" name="ScenarioID"/>
-    <tableColumn id="5" name="Capabilities" dataDxfId="9"/>
+    <tableColumn id="5" name="Capabilities" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="BC_Capabilities" displayName="BC_Capabilities" ref="A2:D4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="ADM_Capabilities" displayName="ADM_Capabilities" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="8"/>
+    <tableColumn id="1" name="Name" dataDxfId="25"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1603,11 +1728,11 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="BC_Threats" displayName="BC_Threats" ref="A7:G9" totalsRowShown="0">
-  <autoFilter ref="A7:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="ADM_Threats" displayName="ADM_Threats" ref="A7:G8" totalsRowShown="0">
+  <autoFilter ref="A7:G8"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="7"/>
-    <tableColumn id="7" name="TComm" dataDxfId="6"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="24"/>
+    <tableColumn id="7" name="TComm" dataDxfId="23"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1619,10 +1744,10 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Privacy_Capabilities" displayName="Privacy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A2:D6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="IM_Capabilities" displayName="IM_Capabilities" ref="A2:D7" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A2:D7"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="2"/>
+    <tableColumn id="1" name="Name" dataDxfId="19"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1632,11 +1757,50 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Privacy_Threats" displayName="Privacy_Threats" ref="A9:G12" totalsRowShown="0">
-  <autoFilter ref="A9:G12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="IM_Threats" displayName="IM_Threats" ref="A10:G22" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A10:G22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="1"/>
-    <tableColumn id="7" name="TComm" dataDxfId="0"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="15"/>
+    <tableColumn id="7" name="TComm" dataDxfId="14"/>
+    <tableColumn id="2" name="TEF"/>
+    <tableColumn id="3" name="TC"/>
+    <tableColumn id="4" name="LM"/>
+    <tableColumn id="6" name="ScenarioID"/>
+    <tableColumn id="5" name="Capabilities" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A11:B13" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="2">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="BC_Capabilities" displayName="BC_Capabilities" ref="A2:D4" totalsRowShown="0">
+  <autoFilter ref="A2:D4"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name" dataDxfId="12"/>
+    <tableColumn id="2" name="DIFF"/>
+    <tableColumn id="5" name="Evidence"/>
+    <tableColumn id="3" name="CapabilityID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="BC_Threats" displayName="BC_Threats" ref="A7:G9" totalsRowShown="0">
+  <autoFilter ref="A7:G9"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Scenario" dataDxfId="11"/>
+    <tableColumn id="7" name="TComm" dataDxfId="10"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1647,12 +1811,74 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Privacy_Capabilities" displayName="Privacy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A2:D6"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="2" name="DIFF"/>
+    <tableColumn id="5" name="Evidence"/>
+    <tableColumn id="3" name="CapabilityID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Privacy_Threats" displayName="Privacy_Threats" ref="A9:G12" totalsRowShown="0">
+  <autoFilter ref="A9:G12"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Scenario" dataDxfId="5"/>
+    <tableColumn id="7" name="TComm" dataDxfId="4"/>
+    <tableColumn id="2" name="TEF"/>
+    <tableColumn id="3" name="TC"/>
+    <tableColumn id="4" name="LM"/>
+    <tableColumn id="6" name="ScenarioID"/>
+    <tableColumn id="5" name="Capabilities"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A16:B18" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="1">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A21:B23" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ISMP_Capabilities" displayName="ISMP_Capabilities" ref="A2:D5" totalsRowShown="0">
+  <autoFilter ref="A2:D5"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name" dataDxfId="78"/>
+    <tableColumn id="4" name="DIFF"/>
+    <tableColumn id="5" name="Evidence"/>
+    <tableColumn id="2" name="CapabilityID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ISMP_Threats" displayName="ISMP_Threats" ref="A8:G9" totalsRowShown="0">
   <autoFilter ref="A8:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="73"/>
-    <tableColumn id="11" name="TComm" dataDxfId="72"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="77"/>
+    <tableColumn id="11" name="TComm" dataDxfId="76"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1663,69 +1889,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="AC_Capabilities" displayName="AC_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="AC_Capabilities" displayName="AC_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="75" headerRowBorderDxfId="74" tableBorderDxfId="73">
   <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="68"/>
-    <tableColumn id="2" name="DIFF"/>
-    <tableColumn id="5" name="Evidence"/>
-    <tableColumn id="3" name="CapabilityID"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="AC_Threats" displayName="AC_Threats" ref="A7:G9" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
-  <autoFilter ref="A7:G9"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="64"/>
-    <tableColumn id="7" name="TComm" dataDxfId="63"/>
-    <tableColumn id="2" name="TEF"/>
-    <tableColumn id="3" name="TC"/>
-    <tableColumn id="4" name="LM"/>
-    <tableColumn id="6" name="ScenarioID"/>
-    <tableColumn id="5" name="Capabilities"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="HR_Capabilites" displayName="HR_Capabilites" ref="A2:D6" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60">
-  <autoFilter ref="A2:D6"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" name="DIFF"/>
-    <tableColumn id="5" name="Evidence"/>
-    <tableColumn id="3" name="CapabilityID"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="HR_Threats" displayName="HR_Threats" ref="A9:G13" totalsRowShown="0">
-  <autoFilter ref="A9:G13"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="58"/>
-    <tableColumn id="7" name="TComm" dataDxfId="57"/>
-    <tableColumn id="2" name="TEF"/>
-    <tableColumn id="3" name="TC"/>
-    <tableColumn id="4" name="LM"/>
-    <tableColumn id="6" name="ScenarioID"/>
-    <tableColumn id="5" name="Capabilities"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Risk_Capabilities" displayName="Risk_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
-  <autoFilter ref="A2:D6"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="53"/>
+    <tableColumn id="1" name="Name" dataDxfId="72"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1735,11 +1903,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Risk_Threats" displayName="Risk_Threats" ref="A9:G13" totalsRowShown="0">
-  <autoFilter ref="A9:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="AC_Threats" displayName="AC_Threats" ref="A7:G9" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69">
+  <autoFilter ref="A7:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="52"/>
-    <tableColumn id="7" name="TComm" dataDxfId="51"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="68"/>
+    <tableColumn id="7" name="TComm" dataDxfId="67"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -2047,10 +2215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,6 +2351,22 @@
       </c>
       <c r="B16" s="5" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2204,6 +2388,8 @@
     <hyperlink ref="B12" location="OPS!A1" display="OPS"/>
     <hyperlink ref="B14" location="IM!A1" display="IM"/>
     <hyperlink ref="B8" location="ORG!A1" display="ORG"/>
+    <hyperlink ref="B18" location="Definitions!A1" display="Definitions"/>
+    <hyperlink ref="B19" location="Reference!A1" display="Reference"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -2240,6 +2426,228 @@
       <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:G6"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C11">
+      <formula1>TEF_Values</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D11">
+      <formula1>TC_Values</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E11">
+      <formula1>LM_Values</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
+      <formula1>DIFF_Values</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2415,12 +2823,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,12 +3073,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3149,12 +3557,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,12 +3709,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3749,12 +4157,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3924,7 +4332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -4153,10 +4561,290 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="13"/>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4318,117 +5006,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4585,12 +5168,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4835,12 +5418,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5086,12 +5669,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5317,12 +5900,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5643,226 +6226,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="75.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:G6"/>
-  </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C11">
-      <formula1>TEF_Values</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D11">
-      <formula1>TC_Values</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E11">
-      <formula1>LM_Values</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
-      <formula1>DIFF_Values</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Correct data validation. Change DIFF labels to text values to match CMM.
</commit_message>
<xml_diff>
--- a/survey/HITRUST Survey Document.xlsx
+++ b/survey/HITRUST Survey Document.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\evaluator\survey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Primary Docs\Google Drive\Heroku\Shared with Trey\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,18 +30,10 @@
     <sheet name="BC" sheetId="17" r:id="rId16"/>
     <sheet name="PRI" sheetId="5" r:id="rId17"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId18"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="DIFF_Values" localSheetId="14">[1]Reference!$A$17:$A$21</definedName>
     <definedName name="DIFF_Values">Reference!$A$17:$A$21</definedName>
-    <definedName name="LM_Values" localSheetId="14">[1]Reference!$A$12:$A$14</definedName>
     <definedName name="LM_Values">Reference!$A$12:$A$14</definedName>
-    <definedName name="sdfs">[1]Reference!$A$17:$A$21</definedName>
-    <definedName name="TC_Values" localSheetId="14">[1]Reference!$A$7:$A$9</definedName>
     <definedName name="TC_Values">Reference!$A$7:$A$9</definedName>
-    <definedName name="TEF_Values" localSheetId="14">[1]Reference!$A$2:$A$4</definedName>
     <definedName name="TEF_Values">Reference!$A$2:$A$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -54,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="226">
   <si>
     <t>Threats</t>
   </si>
@@ -704,9 +696,6 @@
     <t>Threat actor has low capability.</t>
   </si>
   <si>
-    <t>Optimized.</t>
-  </si>
-  <si>
     <t>Tested and reviewed.</t>
   </si>
   <si>
@@ -717,6 +706,24 @@
   </si>
   <si>
     <t>Not performed or performed inconsistently.</t>
+  </si>
+  <si>
+    <t>Optimized. Completely effective. World class.</t>
+  </si>
+  <si>
+    <t>Optimizing</t>
+  </si>
+  <si>
+    <t>Managed</t>
+  </si>
+  <si>
+    <t>Defined</t>
+  </si>
+  <si>
+    <t>Repeatable</t>
+  </si>
+  <si>
+    <t>Initial</t>
   </si>
 </sst>
 </file>
@@ -832,7 +839,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -840,9 +850,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
@@ -852,34 +859,6 @@
     <cellStyle name="Title" xfId="3" builtinId="15"/>
   </cellStyles>
   <dxfs count="79">
-    <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1335,6 +1314,34 @@
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1346,116 +1353,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ORG"/>
-      <sheetName val="Reference"/>
-      <sheetName val="POL"/>
-      <sheetName val="AUD"/>
-      <sheetName val="RISK"/>
-      <sheetName val="PRI"/>
-      <sheetName val="IM"/>
-      <sheetName val="EDU"/>
-      <sheetName val="IMON"/>
-      <sheetName val="OPS"/>
-      <sheetName val="TECH"/>
-      <sheetName val="PHY"/>
-      <sheetName val="ASSET"/>
-      <sheetName val="ACCT"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Frequent</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Occasional</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Rare</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>High</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Medium</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Low</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>High</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Medium</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Low</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>5</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1470,10 +1367,10 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="HR_Capabilites" displayName="HR_Capabilites" ref="A2:D6" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="HR_Capabilites" displayName="HR_Capabilites" ref="A2:D6" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60">
   <autoFilter ref="A2:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="63"/>
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1486,8 +1383,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="HR_Threats" displayName="HR_Threats" ref="A9:G13" totalsRowShown="0">
   <autoFilter ref="A9:G13"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="62"/>
-    <tableColumn id="7" name="TComm" dataDxfId="61"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="58"/>
+    <tableColumn id="7" name="TComm" dataDxfId="57"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1499,10 +1396,10 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Risk_Capabilities" displayName="Risk_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Risk_Capabilities" displayName="Risk_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
   <autoFilter ref="A2:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="57"/>
+    <tableColumn id="1" name="Name" dataDxfId="53"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1515,8 +1412,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Risk_Threats" displayName="Risk_Threats" ref="A9:G13" totalsRowShown="0">
   <autoFilter ref="A9:G13"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="56"/>
-    <tableColumn id="7" name="TComm" dataDxfId="55"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="52"/>
+    <tableColumn id="7" name="TComm" dataDxfId="51"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1531,8 +1428,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Policy_Threats" displayName="Policy_Threats" ref="A9:G12" totalsRowShown="0">
   <autoFilter ref="A9:G12"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="54"/>
-    <tableColumn id="7" name="TComm" dataDxfId="53"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="50"/>
+    <tableColumn id="7" name="TComm" dataDxfId="49"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1544,10 +1441,10 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Policy_Capabilities" displayName="Policy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Policy_Capabilities" displayName="Policy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46">
   <autoFilter ref="A2:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="49"/>
+    <tableColumn id="1" name="Name" dataDxfId="45"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1560,7 +1457,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="ORG_Capabilities" displayName="ORG_Capabilities" ref="A2:D10" totalsRowShown="0">
   <autoFilter ref="A2:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="48"/>
+    <tableColumn id="1" name="Name" dataDxfId="44"/>
     <tableColumn id="4" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="2" name="CapabilityID"/>
@@ -1573,8 +1470,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="ORG_Threats" displayName="ORG_Threats" ref="A13:G18" totalsRowShown="0">
   <autoFilter ref="A13:G18"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="47"/>
-    <tableColumn id="11" name="TComm" dataDxfId="46"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="43"/>
+    <tableColumn id="11" name="TComm" dataDxfId="42"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1589,9 +1486,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="COMP_Capabilities" displayName="COMP_Capabilities" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="45"/>
+    <tableColumn id="1" name="Name" dataDxfId="41"/>
     <tableColumn id="2" name="DIFF"/>
-    <tableColumn id="5" name="Evidence" dataDxfId="44"/>
+    <tableColumn id="5" name="Evidence" dataDxfId="40"/>
     <tableColumn id="3" name="CapabilityID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1602,8 +1499,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="COMP_Threats" displayName="COMP_Threats" ref="A7:G11" totalsRowShown="0">
   <autoFilter ref="A7:G11"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="43"/>
-    <tableColumn id="7" name="TComm" dataDxfId="42"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="39"/>
+    <tableColumn id="7" name="TComm" dataDxfId="38"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1615,7 +1512,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A4:B8" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A4:B8" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="78">
   <sortState ref="A4:B8">
     <sortCondition descending="1" ref="A4:A8"/>
   </sortState>
@@ -1628,10 +1525,10 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Asset_Capabilities" displayName="Asset_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Asset_Capabilities" displayName="Asset_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35">
   <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="38"/>
+    <tableColumn id="1" name="Name" dataDxfId="34"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1641,11 +1538,11 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Asset_Threats" displayName="Asset_Threats" ref="A8:G11" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Asset_Threats" displayName="Asset_Threats" ref="A8:G11" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A8:G11"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="34"/>
-    <tableColumn id="7" name="TComm" dataDxfId="33"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="30"/>
+    <tableColumn id="7" name="TComm" dataDxfId="29"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1660,7 +1557,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Physical_Capabilities" displayName="Physical_Capabilities" ref="A2:D6" totalsRowShown="0">
   <autoFilter ref="A2:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="32"/>
+    <tableColumn id="1" name="Name" dataDxfId="28"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1673,8 +1570,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Physical_Threats" displayName="Physical_Threats" ref="A9:G13" totalsRowShown="0">
   <autoFilter ref="A9:G13"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="31"/>
-    <tableColumn id="7" name="TComm" dataDxfId="30"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="27"/>
+    <tableColumn id="7" name="TComm" dataDxfId="26"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1689,7 +1586,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="OPS_Capabilities" displayName="OPS_Capabilities" ref="A2:D16" totalsRowShown="0">
   <autoFilter ref="A2:D16"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="29"/>
+    <tableColumn id="1" name="Name" dataDxfId="25"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1702,13 +1599,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="OPS_Threats" displayName="OPS_Threats" ref="A19:G27" totalsRowShown="0">
   <autoFilter ref="A19:G27"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="28"/>
-    <tableColumn id="7" name="TComm" dataDxfId="27"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="24"/>
+    <tableColumn id="7" name="TComm" dataDxfId="23"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
     <tableColumn id="6" name="ScenarioID"/>
-    <tableColumn id="5" name="Capabilities" dataDxfId="26"/>
+    <tableColumn id="5" name="Capabilities" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1718,7 +1615,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="ADM_Capabilities" displayName="ADM_Capabilities" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="25"/>
+    <tableColumn id="1" name="Name" dataDxfId="21"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1731,8 +1628,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="ADM_Threats" displayName="ADM_Threats" ref="A7:G8" totalsRowShown="0">
   <autoFilter ref="A7:G8"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="24"/>
-    <tableColumn id="7" name="TComm" dataDxfId="23"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="20"/>
+    <tableColumn id="7" name="TComm" dataDxfId="19"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1744,10 +1641,10 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="IM_Capabilities" displayName="IM_Capabilities" ref="A2:D7" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="IM_Capabilities" displayName="IM_Capabilities" ref="A2:D7" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A2:D7"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="19"/>
+    <tableColumn id="1" name="Name" dataDxfId="15"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1757,23 +1654,23 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="IM_Threats" displayName="IM_Threats" ref="A10:G22" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="IM_Threats" displayName="IM_Threats" ref="A10:G22" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A10:G22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="15"/>
-    <tableColumn id="7" name="TComm" dataDxfId="14"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="11"/>
+    <tableColumn id="7" name="TComm" dataDxfId="10"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
     <tableColumn id="6" name="ScenarioID"/>
-    <tableColumn id="5" name="Capabilities" dataDxfId="13"/>
+    <tableColumn id="5" name="Capabilities" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A11:B13" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A11:B13" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="77">
   <tableColumns count="2">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
@@ -1786,7 +1683,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="BC_Capabilities" displayName="BC_Capabilities" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="12"/>
+    <tableColumn id="1" name="Name" dataDxfId="8"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1799,8 +1696,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="BC_Threats" displayName="BC_Threats" ref="A7:G9" totalsRowShown="0">
   <autoFilter ref="A7:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="11"/>
-    <tableColumn id="7" name="TComm" dataDxfId="10"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="7"/>
+    <tableColumn id="7" name="TComm" dataDxfId="6"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1812,10 +1709,10 @@
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Privacy_Capabilities" displayName="Privacy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Privacy_Capabilities" displayName="Privacy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A2:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="1" name="Name" dataDxfId="2"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1828,8 +1725,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Privacy_Threats" displayName="Privacy_Threats" ref="A9:G12" totalsRowShown="0">
   <autoFilter ref="A9:G12"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="5"/>
-    <tableColumn id="7" name="TComm" dataDxfId="4"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="1"/>
+    <tableColumn id="7" name="TComm" dataDxfId="0"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1841,7 +1738,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A16:B18" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A16:B18" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="76">
   <tableColumns count="2">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
@@ -1851,7 +1748,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A21:B23" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A21:B23" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="75">
   <tableColumns count="2">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
@@ -1864,7 +1761,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ISMP_Capabilities" displayName="ISMP_Capabilities" ref="A2:D5" totalsRowShown="0">
   <autoFilter ref="A2:D5"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="78"/>
+    <tableColumn id="1" name="Name" dataDxfId="74"/>
     <tableColumn id="4" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="2" name="CapabilityID"/>
@@ -1877,8 +1774,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ISMP_Threats" displayName="ISMP_Threats" ref="A8:G9" totalsRowShown="0">
   <autoFilter ref="A8:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="77"/>
-    <tableColumn id="11" name="TComm" dataDxfId="76"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="73"/>
+    <tableColumn id="11" name="TComm" dataDxfId="72"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -1890,10 +1787,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="AC_Capabilities" displayName="AC_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="75" headerRowBorderDxfId="74" tableBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="AC_Capabilities" displayName="AC_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="72"/>
+    <tableColumn id="1" name="Name" dataDxfId="68"/>
     <tableColumn id="2" name="DIFF"/>
     <tableColumn id="5" name="Evidence"/>
     <tableColumn id="3" name="CapabilityID"/>
@@ -1903,11 +1800,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="AC_Threats" displayName="AC_Threats" ref="A7:G9" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="AC_Threats" displayName="AC_Threats" ref="A7:G9" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="A7:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="68"/>
-    <tableColumn id="7" name="TComm" dataDxfId="67"/>
+    <tableColumn id="1" name="Scenario" dataDxfId="64"/>
+    <tableColumn id="7" name="TComm" dataDxfId="63"/>
     <tableColumn id="2" name="TEF"/>
     <tableColumn id="3" name="TC"/>
     <tableColumn id="4" name="LM"/>
@@ -2228,10 +2125,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2418,12 +2315,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2443,8 +2340,8 @@
       <c r="A3" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -2457,8 +2354,8 @@
       <c r="A4" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B4">
-        <v>5</v>
+      <c r="B4" t="s">
+        <v>221</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>69</v>
@@ -2468,15 +2365,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2640,12 +2537,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2665,8 +2562,8 @@
       <c r="A3" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -2679,8 +2576,8 @@
       <c r="A4" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -2693,15 +2590,15 @@
       <c r="A5" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2800,7 +2697,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:G7"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="4">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C11">
       <formula1>TEF_Values</formula1>
     </dataValidation>
@@ -2842,12 +2739,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2867,8 +2764,8 @@
       <c r="A3" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B3">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>223</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -2881,8 +2778,8 @@
       <c r="A4" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>223</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -2895,8 +2792,8 @@
       <c r="A5" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B5">
-        <v>5</v>
+      <c r="B5" t="s">
+        <v>221</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -2909,8 +2806,8 @@
       <c r="A6" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -2920,15 +2817,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3092,12 +2989,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3117,8 +3014,8 @@
       <c r="A3" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B3">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>223</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -3131,8 +3028,8 @@
       <c r="A4" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -3145,8 +3042,8 @@
       <c r="A5" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B5">
-        <v>2</v>
+      <c r="B5" t="s">
+        <v>224</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -3159,8 +3056,8 @@
       <c r="A6" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -3173,8 +3070,8 @@
       <c r="A7" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B7">
-        <v>2</v>
+      <c r="B7" t="s">
+        <v>224</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
@@ -3187,8 +3084,8 @@
       <c r="A8" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B8">
-        <v>2</v>
+      <c r="B8" t="s">
+        <v>224</v>
       </c>
       <c r="C8" t="s">
         <v>69</v>
@@ -3201,8 +3098,8 @@
       <c r="A9" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B9">
-        <v>4</v>
+      <c r="B9" t="s">
+        <v>222</v>
       </c>
       <c r="C9" t="s">
         <v>69</v>
@@ -3215,8 +3112,8 @@
       <c r="A10" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B10">
-        <v>5</v>
+      <c r="B10" t="s">
+        <v>221</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
@@ -3229,8 +3126,8 @@
       <c r="A11" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B11">
-        <v>3</v>
+      <c r="B11" t="s">
+        <v>223</v>
       </c>
       <c r="C11" t="s">
         <v>69</v>
@@ -3243,8 +3140,8 @@
       <c r="A12" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B12">
-        <v>5</v>
+      <c r="B12" t="s">
+        <v>221</v>
       </c>
       <c r="C12" t="s">
         <v>69</v>
@@ -3257,8 +3154,8 @@
       <c r="A13" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B13">
-        <v>3</v>
+      <c r="B13" t="s">
+        <v>223</v>
       </c>
       <c r="C13" t="s">
         <v>69</v>
@@ -3271,8 +3168,8 @@
       <c r="A14" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B14">
-        <v>1</v>
+      <c r="B14" t="s">
+        <v>225</v>
       </c>
       <c r="C14" t="s">
         <v>69</v>
@@ -3285,8 +3182,8 @@
       <c r="A15" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B15">
-        <v>1</v>
+      <c r="B15" t="s">
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>69</v>
@@ -3299,8 +3196,8 @@
       <c r="A16" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B16">
-        <v>1</v>
+      <c r="B16" t="s">
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>69</v>
@@ -3313,15 +3210,15 @@
       <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -3575,12 +3472,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3600,8 +3497,8 @@
       <c r="A3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B3">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>223</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -3614,8 +3511,8 @@
       <c r="A4" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B4">
-        <v>5</v>
+      <c r="B4" t="s">
+        <v>221</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -3625,15 +3522,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3728,12 +3625,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3753,8 +3650,8 @@
       <c r="A3" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -3767,8 +3664,8 @@
       <c r="A4" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -3781,8 +3678,8 @@
       <c r="A5" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B5">
-        <v>4</v>
+      <c r="B5" t="s">
+        <v>222</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -3795,8 +3692,8 @@
       <c r="A6" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B6">
-        <v>4</v>
+      <c r="B6" t="s">
+        <v>222</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -3809,8 +3706,8 @@
       <c r="A7" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B7">
-        <v>5</v>
+      <c r="B7" t="s">
+        <v>221</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
@@ -3820,15 +3717,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4175,12 +4072,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4200,8 +4097,8 @@
       <c r="A3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B3">
-        <v>5</v>
+      <c r="B3" t="s">
+        <v>221</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -4214,8 +4111,8 @@
       <c r="A4" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>223</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -4225,15 +4122,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -4351,12 +4248,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4376,8 +4273,8 @@
       <c r="A3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -4390,8 +4287,8 @@
       <c r="A4" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -4404,8 +4301,8 @@
       <c r="A5" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B5">
-        <v>5</v>
+      <c r="B5" t="s">
+        <v>221</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -4418,8 +4315,8 @@
       <c r="A6" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B6">
-        <v>5</v>
+      <c r="B6" t="s">
+        <v>221</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -4429,15 +4326,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -4569,73 +4466,73 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="81.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="A4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="12" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" s="12" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
     <row r="10" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4643,7 +4540,7 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4651,21 +4548,21 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="7" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4673,7 +4570,7 @@
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="7" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4681,21 +4578,21 @@
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="7" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="7" t="s">
         <v>198</v>
       </c>
     </row>
@@ -4703,7 +4600,7 @@
       <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="7" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4711,7 +4608,7 @@
       <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="8" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4739,10 +4636,13 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4810,28 +4710,28 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
+      <c r="A17" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2</v>
+      <c r="A18" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>3</v>
+      <c r="A19" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
+      <c r="A20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5</v>
+      <c r="A21" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4858,12 +4758,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4883,8 +4783,8 @@
       <c r="A3" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -4897,8 +4797,8 @@
       <c r="A4" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>224</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -4911,8 +4811,8 @@
       <c r="A5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B5">
-        <v>5</v>
+      <c r="B5" t="s">
+        <v>221</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -4922,15 +4822,15 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -5025,12 +4925,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5050,8 +4950,8 @@
       <c r="A3" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -5064,8 +4964,8 @@
       <c r="A4" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>223</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -5075,15 +4975,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -5159,6 +5059,20 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A6:G6"/>
   </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
+      <formula1>DIFF_Values</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C9">
+      <formula1>TEF_Values</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9">
+      <formula1>TC_Values</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E9">
+      <formula1>LM_Values</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
   <tableParts count="2">
@@ -5187,12 +5101,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5212,8 +5126,8 @@
       <c r="A3" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -5226,8 +5140,8 @@
       <c r="A4" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>223</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -5240,8 +5154,8 @@
       <c r="A5" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -5254,8 +5168,8 @@
       <c r="A6" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="B6" t="s">
+        <v>224</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -5265,15 +5179,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -5438,12 +5352,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5463,8 +5377,8 @@
       <c r="A3" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B3">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -5477,8 +5391,8 @@
       <c r="A4" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>223</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -5491,8 +5405,8 @@
       <c r="A5" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B5">
-        <v>5</v>
+      <c r="B5" t="s">
+        <v>221</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -5505,8 +5419,8 @@
       <c r="A6" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B6">
-        <v>5</v>
+      <c r="B6" t="s">
+        <v>221</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -5516,15 +5430,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -5689,12 +5603,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5714,8 +5628,8 @@
       <c r="A3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -5728,8 +5642,8 @@
       <c r="A4" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B4">
-        <v>5</v>
+      <c r="B4" t="s">
+        <v>221</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -5742,8 +5656,8 @@
       <c r="A5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B5">
-        <v>2</v>
+      <c r="B5" t="s">
+        <v>224</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -5756,8 +5670,8 @@
       <c r="A6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="B6" t="s">
+        <v>224</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -5770,15 +5684,15 @@
       <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -5918,12 +5832,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5943,8 +5857,8 @@
       <c r="A3" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B3">
-        <v>5</v>
+      <c r="B3" t="s">
+        <v>221</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -5957,8 +5871,8 @@
       <c r="A4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>224</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -5971,8 +5885,8 @@
       <c r="A5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B5">
-        <v>4</v>
+      <c r="B5" t="s">
+        <v>222</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -5985,8 +5899,8 @@
       <c r="A6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -5999,8 +5913,8 @@
       <c r="A7" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B7">
-        <v>4</v>
+      <c r="B7" t="s">
+        <v>222</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
@@ -6013,8 +5927,8 @@
       <c r="A8" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B8">
-        <v>4</v>
+      <c r="B8" t="s">
+        <v>222</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>69</v>
@@ -6027,8 +5941,8 @@
       <c r="A9" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B9">
-        <v>2</v>
+      <c r="B9" t="s">
+        <v>224</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>69</v>
@@ -6041,8 +5955,8 @@
       <c r="A10" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B10">
-        <v>2</v>
+      <c r="B10" t="s">
+        <v>224</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>69</v>
@@ -6052,15 +5966,15 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
Update DIFF settings to include ranked labels
</commit_message>
<xml_diff>
--- a/survey/HITRUST Survey Document.xlsx
+++ b/survey/HITRUST Survey Document.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Primary Docs\Google Drive\Heroku\Shared with Trey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\evaluator\survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -711,19 +711,19 @@
     <t>Optimized. Completely effective. World class.</t>
   </si>
   <si>
-    <t>Optimizing</t>
-  </si>
-  <si>
-    <t>Managed</t>
-  </si>
-  <si>
-    <t>Defined</t>
-  </si>
-  <si>
-    <t>Repeatable</t>
-  </si>
-  <si>
-    <t>Initial</t>
+    <t>4 - Managed</t>
+  </si>
+  <si>
+    <t>5 - Optimized</t>
+  </si>
+  <si>
+    <t>3 - Defined</t>
+  </si>
+  <si>
+    <t>2 - Repeatable</t>
+  </si>
+  <si>
+    <t>1 - Initial</t>
   </si>
 </sst>
 </file>
@@ -2355,7 +2355,7 @@
         <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>69</v>
@@ -2793,7 +2793,7 @@
         <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -3099,7 +3099,7 @@
         <v>158</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C9" t="s">
         <v>69</v>
@@ -3113,7 +3113,7 @@
         <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
@@ -3141,7 +3141,7 @@
         <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C12" t="s">
         <v>69</v>
@@ -3512,7 +3512,7 @@
         <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -3679,7 +3679,7 @@
         <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -3693,7 +3693,7 @@
         <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -3707,7 +3707,7 @@
         <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
@@ -4098,7 +4098,7 @@
         <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -4302,7 +4302,7 @@
         <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -4316,7 +4316,7 @@
         <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -4466,7 +4466,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="81.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>220</v>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>216</v>
@@ -4635,13 +4635,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -4726,12 +4726,12 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4812,7 +4812,7 @@
         <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -5406,7 +5406,7 @@
         <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -5420,7 +5420,7 @@
         <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -5643,7 +5643,7 @@
         <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -5858,7 +5858,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -5886,7 +5886,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -5914,7 +5914,7 @@
         <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
@@ -5928,7 +5928,7 @@
         <v>123</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Make the sample data a bit more realistic rather than purely random
</commit_message>
<xml_diff>
--- a/survey/HITRUST Survey Document.xlsx
+++ b/survey/HITRUST Survey Document.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="228">
   <si>
     <t>Threats</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Unauthorized access to or use of information and systems</t>
-  </si>
-  <si>
     <t>Evidence</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Increased negligence by workforce members due to lack of appropriate delegated authority and security support.</t>
   </si>
   <si>
-    <t>The security functions implements a security strategy that has unanticipated consequences on the insitution, interfering with other stated business objectives.</t>
-  </si>
-  <si>
     <t>Inadequate human resources are available to execute the strategic security plan.</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>Through insufficient training, workforce members cannot identify (or fail to report) potential information security incidents, resulting in loss from undetected attacks.</t>
   </si>
   <si>
-    <t>Successful social engineering attacks resulting in information or financial loss.</t>
-  </si>
-  <si>
     <t>Business disruption and non-recovery of data.</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>Loss of information assets due to misclassification and non-classification.</t>
   </si>
   <si>
-    <t>No accountability for critical information and systems results in inappropriate control and inventory.</t>
-  </si>
-  <si>
     <t>Unauthorized access to or use of information and systems results in inappropriate use by internal users.</t>
   </si>
   <si>
@@ -231,15 +219,9 @@
     <t>Organizational Workforce</t>
   </si>
   <si>
-    <t>New and changing regulations are not adopted on Organizational IT systems.</t>
-  </si>
-  <si>
     <t>Organizational IT</t>
   </si>
   <si>
-    <t>Security failure or instability of providers or partners results in disclosure of Organizational data.</t>
-  </si>
-  <si>
     <t>Organizational Partners</t>
   </si>
   <si>
@@ -579,9 +561,6 @@
     <t>29, 30, 31, 60</t>
   </si>
   <si>
-    <t>1, 3, 5, 7, 32, 13, 14, 15, 16</t>
-  </si>
-  <si>
     <t>8, 13</t>
   </si>
   <si>
@@ -603,24 +582,15 @@
     <t>Unknown attack intelligence results in undetected events.</t>
   </si>
   <si>
-    <t>32, 33, 34, 35, 36</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unknown incidence of security breach </t>
   </si>
   <si>
-    <t>Lack of monitoring demonstrate failure to take due care, resulting in non-compliance with associated laws and regulations.</t>
-  </si>
-  <si>
     <t>External Auditor</t>
   </si>
   <si>
     <t>Destruction, misuse, or modification of information assets through breach of technical controls.</t>
   </si>
   <si>
-    <t>46, 47, 48, 49, 50</t>
-  </si>
-  <si>
     <t>Eroding network boundaries result in lack of defenses on systems.</t>
   </si>
   <si>
@@ -724,6 +694,42 @@
   </si>
   <si>
     <t>1 - Initial</t>
+  </si>
+  <si>
+    <t>Lack of monitoring demonstrates failure to take due care, resulting in non-compliance with associated laws and regulations.</t>
+  </si>
+  <si>
+    <t>Unauthorized access to or use of information and systems.</t>
+  </si>
+  <si>
+    <t>30, 31, 60</t>
+  </si>
+  <si>
+    <t>Successful social engineering attacks result in information or financial loss.</t>
+  </si>
+  <si>
+    <t>Security failure or instability of providers or partners results in disclosure of organizational data.</t>
+  </si>
+  <si>
+    <t>The security function implements a security strategy that has unanticipated consequences on the insitution, interfering with other stated business objectives.</t>
+  </si>
+  <si>
+    <t>1, 7, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>1, 3, 5, 7, 32, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>1, 5, 7, 32, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>New or changing privacy regulations are not implemented in organizational IT systems.</t>
+  </si>
+  <si>
+    <t>Lack of accountability for critical information and systems results in inappropriate control and inventory.</t>
+  </si>
+  <si>
+    <t>33, 34, 35, 36</t>
   </si>
 </sst>
 </file>
@@ -2126,144 +2132,144 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2316,7 +2322,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2330,21 +2336,21 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -2352,13 +2358,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>13</v>
@@ -2377,10 +2383,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -2392,102 +2398,102 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>225</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
       <c r="F8">
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2538,7 +2544,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2552,21 +2558,21 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>56</v>
@@ -2574,13 +2580,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>39</v>
@@ -2602,10 +2608,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
@@ -2617,79 +2623,79 @@
         <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
         <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
       </c>
       <c r="F9">
         <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2740,7 +2746,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2754,21 +2760,21 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>52</v>
@@ -2776,13 +2782,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>53</v>
@@ -2790,13 +2796,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>54</v>
@@ -2804,13 +2810,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>55</v>
@@ -2829,10 +2835,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -2844,102 +2850,102 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11">
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2990,7 +2996,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -3004,21 +3010,21 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>37</v>
@@ -3026,13 +3032,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>40</v>
@@ -3040,13 +3046,13 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>42</v>
@@ -3054,13 +3060,13 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>43</v>
@@ -3068,13 +3074,13 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>46</v>
@@ -3082,13 +3088,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D8">
         <v>47</v>
@@ -3096,13 +3102,13 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>48</v>
@@ -3110,13 +3116,13 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D10">
         <v>49</v>
@@ -3124,13 +3130,13 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -3138,13 +3144,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D12">
         <v>51</v>
@@ -3152,13 +3158,13 @@
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D13">
         <v>33</v>
@@ -3166,13 +3172,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D14">
         <v>34</v>
@@ -3180,13 +3186,13 @@
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D15">
         <v>35</v>
@@ -3194,13 +3200,13 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D16">
         <v>36</v>
@@ -3222,10 +3228,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -3237,194 +3243,194 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F20">
         <v>32</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21">
         <v>33</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22">
         <v>34</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
         <v>10</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
       </c>
       <c r="F23">
         <v>35</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24">
         <v>36</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25">
         <v>28</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
         <v>10</v>
-      </c>
-      <c r="E26" t="s">
-        <v>11</v>
       </c>
       <c r="F26">
         <v>29</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F27">
         <v>30</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3473,7 +3479,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3487,21 +3493,21 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>38</v>
@@ -3509,13 +3515,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>44</v>
@@ -3534,10 +3540,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -3549,33 +3555,33 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3626,7 +3632,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -3640,21 +3646,21 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -3662,13 +3668,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>26</v>
@@ -3676,13 +3682,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>27</v>
@@ -3690,13 +3696,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>28</v>
@@ -3704,13 +3710,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>59</v>
@@ -3729,10 +3735,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
@@ -3744,165 +3750,165 @@
         <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11">
         <v>19</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>20</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>21</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F17">
         <v>52</v>
@@ -3913,19 +3919,19 @@
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
       </c>
       <c r="F18">
         <v>53</v>
@@ -3936,94 +3942,94 @@
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19">
         <v>37</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20">
         <v>38</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
         <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
       </c>
       <c r="F21">
         <v>39</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22">
         <v>40</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -4073,7 +4079,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -4087,21 +4093,21 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>41</v>
@@ -4109,13 +4115,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>45</v>
@@ -4134,10 +4140,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -4149,56 +4155,56 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8">
         <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -4249,7 +4255,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4263,21 +4269,21 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>21</v>
@@ -4285,13 +4291,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>22</v>
@@ -4299,13 +4305,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>23</v>
@@ -4313,13 +4319,13 @@
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>24</v>
@@ -4338,10 +4344,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -4353,79 +4359,79 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4472,144 +4478,144 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4651,17 +4657,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -4671,17 +4677,17 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -4691,17 +4697,17 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -4711,27 +4717,27 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -4759,7 +4765,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4773,21 +4779,21 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -4795,13 +4801,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -4809,13 +4815,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -4834,10 +4840,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -4849,33 +4855,33 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -4926,7 +4932,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4940,21 +4946,21 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>57</v>
@@ -4962,13 +4968,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>58</v>
@@ -4987,10 +4993,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -5002,56 +5008,56 @@
         <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>217</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -5102,7 +5108,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5116,21 +5122,21 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>29</v>
@@ -5138,13 +5144,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>30</v>
@@ -5152,13 +5158,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>31</v>
@@ -5166,13 +5172,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -5191,10 +5197,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -5206,102 +5212,102 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
         <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
       </c>
       <c r="F10">
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>219</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -5353,7 +5359,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5367,21 +5373,21 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>17</v>
@@ -5389,13 +5395,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -5403,13 +5409,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>19</v>
@@ -5417,13 +5423,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -5442,10 +5448,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -5457,102 +5463,102 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -5604,7 +5610,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5618,21 +5624,21 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>9</v>
@@ -5640,13 +5646,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -5654,13 +5660,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -5668,13 +5674,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>12</v>
@@ -5696,10 +5702,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -5711,79 +5717,79 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11">
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
         <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
       </c>
       <c r="F12">
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -5833,7 +5839,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5847,21 +5853,21 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -5869,13 +5875,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -5883,13 +5889,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -5897,13 +5903,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -5911,13 +5917,13 @@
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>32</v>
@@ -5925,13 +5931,13 @@
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D8">
         <v>14</v>
@@ -5939,13 +5945,13 @@
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -5953,13 +5959,13 @@
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D10">
         <v>16</v>
@@ -5978,10 +5984,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -5993,125 +5999,125 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F17">
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>177</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>221</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
       </c>
       <c r="F18">
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clarify wording on a couple of lines.
</commit_message>
<xml_diff>
--- a/survey/HITRUST Survey Document.xlsx
+++ b/survey/HITRUST Survey Document.xlsx
@@ -105,18 +105,9 @@
     <t>ScenarioID</t>
   </si>
   <si>
-    <t>Budget does not adequately support information security strategic plan.</t>
-  </si>
-  <si>
-    <t>Competing priorities within the institution results in inability to execute the strategic security plan.</t>
-  </si>
-  <si>
     <t>Increased negligence by workforce members due to lack of appropriate delegated authority and security support.</t>
   </si>
   <si>
-    <t>Inadequate human resources are available to execute the strategic security plan.</t>
-  </si>
-  <si>
     <t>External auditors find compliance issues with regulations and standards not identified via internal processes.</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>Uncontrolled aggregation, proliferation, and use of data.</t>
   </si>
   <si>
-    <t>Lack of incident handling results in noncompliance with laws, regulations, and contractual agreements</t>
-  </si>
-  <si>
     <t>Failure to address security incidents results in reputation loss.</t>
   </si>
   <si>
@@ -174,9 +162,6 @@
     <t>Inability to respond to HR investigations results in avoidable adverse judgements.</t>
   </si>
   <si>
-    <t>Changing cultures with use of data with insufficient education results in privacy violations.</t>
-  </si>
-  <si>
     <t>Through insufficient training, workforce members cannot identify (or fail to report) potential information security incidents, resulting in loss from undetected attacks.</t>
   </si>
   <si>
@@ -195,9 +180,6 @@
     <t>Breach through technical controls results in reportable significant unauthorized disclosure of data.</t>
   </si>
   <si>
-    <t>Changed or adding software without authorization resulting in system performance or data disclosure.</t>
-  </si>
-  <si>
     <t>Theft or loss of physical assets.</t>
   </si>
   <si>
@@ -369,9 +351,6 @@
     <t>Misuse of information assets or user errors (data entry errors, omissions, inadvertent acts or carelessness).</t>
   </si>
   <si>
-    <t>Results of the risk assessments, including any residual risks, are acknowledged by the risk owners.</t>
-  </si>
-  <si>
     <t>Risk assessments are completed on all critical applications, systems, and networks on a periodic basis.</t>
   </si>
   <si>
@@ -522,9 +501,6 @@
     <t>Intrusion detection mechanism is defined, implemented, and maintained.</t>
   </si>
   <si>
-    <t>Baseline measurement process for application, system, and network activity is defined, implemented, and maintained.</t>
-  </si>
-  <si>
     <t>Information Security Incident Management</t>
   </si>
   <si>
@@ -534,9 +510,6 @@
     <t>An incident management process is defined, implemented, and maintained.</t>
   </si>
   <si>
-    <t>Establish working relationships with third party contracted services, counter-intelligence experts, regional organizations, and researchers working in the field of incident response.</t>
-  </si>
-  <si>
     <t>Forensic investigation capabilities are established and available for incident response.</t>
   </si>
   <si>
@@ -546,9 +519,6 @@
     <t>A process exists and is implemented for performing litigation holds.</t>
   </si>
   <si>
-    <t>Undetected and unremediate security incidents results in unmitigated access.</t>
-  </si>
-  <si>
     <t>Organization of Information Security</t>
   </si>
   <si>
@@ -711,9 +681,6 @@
     <t>Security failure or instability of providers or partners results in disclosure of organizational data.</t>
   </si>
   <si>
-    <t>The security function implements a security strategy that has unanticipated consequences on the insitution, interfering with other stated business objectives.</t>
-  </si>
-  <si>
     <t>1, 7, 14, 15, 16</t>
   </si>
   <si>
@@ -730,6 +697,39 @@
   </si>
   <si>
     <t>33, 34, 35, 36</t>
+  </si>
+  <si>
+    <t>Undetected and unremediated security incidents result in unmitigated access.</t>
+  </si>
+  <si>
+    <t>Working relationships are established with third party contracted services, counter-intelligence experts, regional organizations, and researchers working in the field of incident response.</t>
+  </si>
+  <si>
+    <t>Lack of incident handling results in noncompliance with laws, regulations, and contractual agreements.</t>
+  </si>
+  <si>
+    <t>Baseline measurement processes for application, system, and network activity are defined, implemented, and maintained.</t>
+  </si>
+  <si>
+    <t>Changing or adding software without authorization results in system performance or data disclosure.</t>
+  </si>
+  <si>
+    <t>Budget does not adequately support the information security strategic plan.</t>
+  </si>
+  <si>
+    <t>Inadequate human resources are available to execute the informaton security strategic security plan.</t>
+  </si>
+  <si>
+    <t>Competing priorities within the institution results in inability to execute the information security strategic security plan.</t>
+  </si>
+  <si>
+    <t>The information security function implements a strategy that has unanticipated consequences on the insitution, interfering with other stated business objectives.</t>
+  </si>
+  <si>
+    <t>Results of risk assessments, including any residual risks exposures, are acknowledged by the risk owners.</t>
+  </si>
+  <si>
+    <t>Changing cultural norms on the use of data combined with insufficient education results in privacy violations.</t>
   </si>
 </sst>
 </file>
@@ -1544,8 +1544,8 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Asset_Threats" displayName="Asset_Threats" ref="A8:G11" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="A8:G11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Asset_Threats" displayName="Asset_Threats" ref="A7:G10" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
+  <autoFilter ref="A7:G10"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Scenario" dataDxfId="30"/>
     <tableColumn id="7" name="TComm" dataDxfId="29"/>
@@ -2132,144 +2132,144 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2307,7 +2307,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,7 +2322,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2339,18 +2339,18 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>13</v>
@@ -2401,15 +2401,15 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -2424,15 +2424,15 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -2447,15 +2447,15 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -2470,15 +2470,15 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2493,7 +2493,7 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2526,7 +2526,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -2544,7 +2544,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2561,18 +2561,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>56</v>
@@ -2580,13 +2580,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>39</v>
@@ -2595,122 +2595,122 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+    <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>64</v>
+      <c r="G7" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
       <c r="F9">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>121</v>
+        <v>215</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11">
-        <v>47</v>
-      </c>
-      <c r="G11" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A6:G6"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C10">
       <formula1>TEF_Values</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D10">
       <formula1>TC_Values</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E10">
       <formula1>LM_Values</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B5">
@@ -2746,7 +2746,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2763,18 +2763,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>52</v>
@@ -2782,13 +2782,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>53</v>
@@ -2796,13 +2796,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>54</v>
@@ -2810,13 +2810,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>55</v>
@@ -2853,12 +2853,12 @@
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>14</v>
@@ -2876,12 +2876,12 @@
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
@@ -2899,15 +2899,15 @@
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2922,12 +2922,12 @@
         <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>14</v>
@@ -2945,7 +2945,7 @@
         <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2996,7 +2996,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -3013,18 +3013,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>37</v>
@@ -3032,13 +3032,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>40</v>
@@ -3046,13 +3046,13 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>42</v>
@@ -3060,13 +3060,13 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>43</v>
@@ -3074,13 +3074,13 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>46</v>
@@ -3088,13 +3088,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>47</v>
@@ -3102,13 +3102,13 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>48</v>
@@ -3116,13 +3116,13 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D10">
         <v>49</v>
@@ -3130,13 +3130,13 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -3144,13 +3144,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D12">
         <v>51</v>
@@ -3158,13 +3158,13 @@
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="B13" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>33</v>
@@ -3172,13 +3172,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D14">
         <v>34</v>
@@ -3186,13 +3186,13 @@
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D15">
         <v>35</v>
@@ -3200,13 +3200,13 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D16">
         <v>36</v>
@@ -3246,15 +3246,15 @@
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>49</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -3269,12 +3269,12 @@
         <v>32</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -3292,12 +3292,12 @@
         <v>33</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
@@ -3315,12 +3315,12 @@
         <v>34</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -3338,15 +3338,15 @@
         <v>35</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -3361,12 +3361,12 @@
         <v>36</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>14</v>
@@ -3384,12 +3384,12 @@
         <v>28</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>14</v>
@@ -3407,15 +3407,15 @@
         <v>29</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -3430,7 +3430,7 @@
         <v>30</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3479,7 +3479,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3496,18 +3496,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>38</v>
@@ -3515,13 +3515,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>44</v>
@@ -3558,12 +3558,12 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
@@ -3581,7 +3581,7 @@
         <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3632,7 +3632,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -3649,32 +3649,32 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>26</v>
@@ -3682,13 +3682,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>27</v>
@@ -3696,13 +3696,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>28</v>
@@ -3710,13 +3710,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>59</v>
@@ -3753,15 +3753,15 @@
         <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -3776,15 +3776,15 @@
         <v>19</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>219</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -3799,15 +3799,15 @@
         <v>20</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -3822,12 +3822,12 @@
         <v>21</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>14</v>
@@ -3845,12 +3845,12 @@
         <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
@@ -3868,15 +3868,15 @@
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -3891,15 +3891,15 @@
         <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3919,10 +3919,10 @@
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -3942,7 +3942,7 @@
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>14</v>
@@ -3960,12 +3960,12 @@
         <v>37</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>14</v>
@@ -3983,12 +3983,12 @@
         <v>38</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>14</v>
@@ -4006,15 +4006,15 @@
         <v>39</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -4029,7 +4029,7 @@
         <v>40</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4037,7 +4037,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A9:G9"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B7">
       <formula1>DIFF_Values</formula1>
     </dataValidation>
@@ -4079,7 +4079,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -4096,18 +4096,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>41</v>
@@ -4115,13 +4115,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>45</v>
@@ -4158,12 +4158,12 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>16</v>
@@ -4181,15 +4181,15 @@
         <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -4204,7 +4204,7 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4255,7 +4255,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4272,18 +4272,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>21</v>
@@ -4291,13 +4291,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>22</v>
@@ -4305,13 +4305,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>23</v>
@@ -4319,13 +4319,13 @@
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>24</v>
@@ -4362,15 +4362,15 @@
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -4385,15 +4385,15 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -4408,15 +4408,15 @@
         <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -4431,7 +4431,7 @@
         <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4478,59 +4478,59 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B10" s="11"/>
     </row>
@@ -4539,7 +4539,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4547,7 +4547,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4555,12 +4555,12 @@
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B15" s="11"/>
     </row>
@@ -4569,7 +4569,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -4577,7 +4577,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -4585,12 +4585,12 @@
         <v>8</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B20" s="11"/>
     </row>
@@ -4599,7 +4599,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -4607,7 +4607,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4615,7 +4615,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4717,27 +4717,27 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -4765,7 +4765,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4782,18 +4782,18 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -4801,13 +4801,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -4815,13 +4815,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -4858,15 +4858,15 @@
         <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -4881,7 +4881,7 @@
         <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -4932,7 +4932,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4949,18 +4949,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>57</v>
@@ -4968,13 +4968,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>58</v>
@@ -5011,15 +5011,15 @@
         <v>18</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -5034,15 +5034,15 @@
         <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -5057,7 +5057,7 @@
         <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -5108,7 +5108,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5125,18 +5125,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>29</v>
@@ -5144,13 +5144,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>30</v>
@@ -5158,13 +5158,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>31</v>
@@ -5172,13 +5172,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -5215,15 +5215,15 @@
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>227</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -5238,15 +5238,15 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -5261,15 +5261,15 @@
         <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -5284,12 +5284,12 @@
         <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>14</v>
@@ -5307,7 +5307,7 @@
         <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -5359,7 +5359,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5376,18 +5376,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>17</v>
@@ -5395,13 +5395,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -5409,13 +5409,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>19</v>
@@ -5423,13 +5423,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -5466,15 +5466,15 @@
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -5489,15 +5489,15 @@
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -5512,15 +5512,15 @@
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -5535,15 +5535,15 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -5558,7 +5558,7 @@
         <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -5610,7 +5610,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5627,18 +5627,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>9</v>
@@ -5646,13 +5646,13 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -5660,13 +5660,13 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -5674,13 +5674,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>12</v>
@@ -5720,15 +5720,15 @@
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -5743,15 +5743,15 @@
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -5766,15 +5766,15 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -5789,7 +5789,7 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -5839,7 +5839,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5856,18 +5856,18 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -5875,13 +5875,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -5889,13 +5889,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -5903,13 +5903,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -5917,13 +5917,13 @@
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>32</v>
@@ -5931,13 +5931,13 @@
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>14</v>
@@ -5945,13 +5945,13 @@
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -5959,13 +5959,13 @@
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D10">
         <v>16</v>
@@ -6002,15 +6002,15 @@
         <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>223</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -6025,15 +6025,15 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>19</v>
+        <v>222</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -6048,15 +6048,15 @@
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>20</v>
+        <v>224</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -6071,15 +6071,15 @@
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -6094,15 +6094,15 @@
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -6117,7 +6117,7 @@
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>